<commit_message>
Tableau comparatif word et Rmarkdown
</commit_message>
<xml_diff>
--- a/data/biometry_2014_ew.xlsx
+++ b/data/biometry_2014_ew.xlsx
@@ -1,15 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathildevion 1/VirtualBox VMs/SciViews Box 2018a/shared/projects/sdd1_biometry-elisa-eva-marie-mathilde/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3EC67E-5C24-244B-B3F7-603608D6E484}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="27760" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="biometry_2014" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">biometry_2014!$D$2:$D$165</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">biometry_2014!$E$2:$E$165</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -529,8 +539,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,11 +577,1868 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Taille</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> en fonction du poids</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>biometry_2014!$D$2:$D$165</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="164"/>
+                <c:pt idx="0">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>52.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>66.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>87.5</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>76.5</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>73.8</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>53.5</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>67.5</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>70.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>74.2</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>59.1</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>73.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>61.5</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>50.5</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>biometry_2014!$E$2:$E$165</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="164"/>
+                <c:pt idx="0">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>173.2</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>189</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9548-AD45-88ED-0ECDA14A9A34}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="780003328"/>
+        <c:axId val="832470816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="780003328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="832470816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="832470816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="780003328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Graphique 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0A547A9-4C40-5248-B3B6-14280278C721}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -613,7 +2480,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -645,9 +2512,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -679,6 +2564,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -854,14 +2757,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E165"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -884,7 +2789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -907,7 +2812,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -930,7 +2835,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -953,7 +2858,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -976,7 +2881,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -999,7 +2904,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1022,7 +2927,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1045,7 +2950,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1068,7 +2973,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1091,7 +2996,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1114,7 +3019,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1131,13 +3036,13 @@
         <v>171</v>
       </c>
       <c r="F12">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="G12">
         <v>2013</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1160,7 +3065,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1183,7 +3088,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1206,7 +3111,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1229,7 +3134,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1246,13 +3151,13 @@
         <v>165</v>
       </c>
       <c r="F17">
-        <v>16.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G17">
         <v>2013</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1275,7 +3180,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1298,7 +3203,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1321,7 +3226,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1344,7 +3249,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1367,7 +3272,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1390,7 +3295,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1413,7 +3318,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1436,7 +3341,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1459,7 +3364,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1482,7 +3387,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1505,7 +3410,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1528,7 +3433,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1551,7 +3456,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +3479,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1597,7 +3502,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1620,7 +3525,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1643,7 +3548,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1666,7 +3571,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -1689,7 +3594,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1712,7 +3617,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -1735,7 +3640,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1758,7 +3663,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1781,7 +3686,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1804,7 +3709,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1827,7 +3732,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1850,7 +3755,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1873,7 +3778,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1890,13 +3795,13 @@
         <v>172</v>
       </c>
       <c r="F45">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="G45">
         <v>2013</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -1913,13 +3818,13 @@
         <v>162</v>
       </c>
       <c r="F46">
-        <v>16.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="G46">
         <v>2013</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -1936,13 +3841,13 @@
         <v>182</v>
       </c>
       <c r="F47">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="G47">
         <v>2013</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -1965,7 +3870,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -1988,7 +3893,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -2011,7 +3916,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -2034,7 +3939,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -2057,7 +3962,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -2080,7 +3985,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -2103,7 +4008,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -2126,7 +4031,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -2149,7 +4054,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -2172,7 +4077,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -2195,7 +4100,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -2218,7 +4123,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -2241,7 +4146,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -2264,7 +4169,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -2287,7 +4192,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -2310,7 +4215,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -2330,7 +4235,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -2350,7 +4255,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -2373,7 +4278,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -2396,7 +4301,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -2419,7 +4324,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -2442,7 +4347,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -2465,7 +4370,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -2488,7 +4393,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -2511,7 +4416,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -2534,7 +4439,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -2557,7 +4462,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -2580,7 +4485,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -2603,7 +4508,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -2626,7 +4531,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -2649,7 +4554,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -2672,7 +4577,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -2695,7 +4600,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -2718,7 +4623,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -2741,7 +4646,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -2764,7 +4669,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -2787,7 +4692,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>7</v>
       </c>
@@ -2810,7 +4715,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -2821,7 +4726,7 @@
         <v>1995</v>
       </c>
       <c r="D86">
-        <v>66.6</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="E86">
         <v>175</v>
@@ -2833,7 +4738,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>12</v>
       </c>
@@ -2856,7 +4761,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>12</v>
       </c>
@@ -2879,7 +4784,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -2902,7 +4807,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>12</v>
       </c>
@@ -2925,7 +4830,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>12</v>
       </c>
@@ -2948,7 +4853,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>7</v>
       </c>
@@ -2971,7 +4876,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>7</v>
       </c>
@@ -2994,7 +4899,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>7</v>
       </c>
@@ -3017,7 +4922,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>12</v>
       </c>
@@ -3040,7 +4945,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>12</v>
       </c>
@@ -3063,7 +4968,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -3086,7 +4991,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>12</v>
       </c>
@@ -3109,7 +5014,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -3132,7 +5037,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>7</v>
       </c>
@@ -3155,7 +5060,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>12</v>
       </c>
@@ -3178,7 +5083,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -3201,7 +5106,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -3224,7 +5129,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>12</v>
       </c>
@@ -3247,7 +5152,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>12</v>
       </c>
@@ -3270,7 +5175,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>12</v>
       </c>
@@ -3293,7 +5198,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>7</v>
       </c>
@@ -3316,7 +5221,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>12</v>
       </c>
@@ -3339,7 +5244,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>7</v>
       </c>
@@ -3362,7 +5267,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>12</v>
       </c>
@@ -3385,7 +5290,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>7</v>
       </c>
@@ -3408,7 +5313,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>7</v>
       </c>
@@ -3431,7 +5336,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -3454,7 +5359,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>12</v>
       </c>
@@ -3477,7 +5382,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>12</v>
       </c>
@@ -3500,7 +5405,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>7</v>
       </c>
@@ -3523,7 +5428,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>12</v>
       </c>
@@ -3546,7 +5451,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>12</v>
       </c>
@@ -3569,7 +5474,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>12</v>
       </c>
@@ -3592,7 +5497,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>12</v>
       </c>
@@ -3615,7 +5520,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -3638,7 +5543,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>7</v>
       </c>
@@ -3661,7 +5566,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>7</v>
       </c>
@@ -3684,7 +5589,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>7</v>
       </c>
@@ -3707,7 +5612,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -3724,13 +5629,13 @@
         <v>170</v>
       </c>
       <c r="F125">
-        <v>16.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="G125">
         <v>2014</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>7</v>
       </c>
@@ -3753,7 +5658,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>7</v>
       </c>
@@ -3770,13 +5675,13 @@
         <v>180</v>
       </c>
       <c r="F127">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="G127">
         <v>2014</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>7</v>
       </c>
@@ -3799,7 +5704,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>12</v>
       </c>
@@ -3822,7 +5727,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>7</v>
       </c>
@@ -3845,7 +5750,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>12</v>
       </c>
@@ -3868,7 +5773,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>7</v>
       </c>
@@ -3891,7 +5796,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>12</v>
       </c>
@@ -3914,7 +5819,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>12</v>
       </c>
@@ -3937,7 +5842,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>12</v>
       </c>
@@ -3960,7 +5865,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>7</v>
       </c>
@@ -3983,7 +5888,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>7</v>
       </c>
@@ -4006,7 +5911,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>12</v>
       </c>
@@ -4029,7 +5934,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>12</v>
       </c>
@@ -4040,7 +5945,7 @@
         <v>1969</v>
       </c>
       <c r="D139">
-        <v>70.1</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="E139">
         <v>164</v>
@@ -4052,7 +5957,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>7</v>
       </c>
@@ -4075,7 +5980,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>12</v>
       </c>
@@ -4098,7 +6003,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>7</v>
       </c>
@@ -4109,7 +6014,7 @@
         <v>1995</v>
       </c>
       <c r="D142">
-        <v>73.6</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="E142">
         <v>192</v>
@@ -4121,7 +6026,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>12</v>
       </c>
@@ -4144,7 +6049,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>7</v>
       </c>
@@ -4167,7 +6072,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -4190,7 +6095,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>7</v>
       </c>
@@ -4213,7 +6118,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>7</v>
       </c>
@@ -4236,7 +6141,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>12</v>
       </c>
@@ -4259,7 +6164,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>7</v>
       </c>
@@ -4282,7 +6187,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>7</v>
       </c>
@@ -4305,7 +6210,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>12</v>
       </c>
@@ -4328,7 +6233,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>7</v>
       </c>
@@ -4351,7 +6256,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>7</v>
       </c>
@@ -4374,7 +6279,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>12</v>
       </c>
@@ -4397,7 +6302,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>7</v>
       </c>
@@ -4420,7 +6325,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>7</v>
       </c>
@@ -4443,7 +6348,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>7</v>
       </c>
@@ -4466,7 +6371,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>12</v>
       </c>
@@ -4489,7 +6394,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>12</v>
       </c>
@@ -4512,7 +6417,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>12</v>
       </c>
@@ -4535,7 +6440,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>7</v>
       </c>
@@ -4558,7 +6463,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>12</v>
       </c>
@@ -4581,7 +6486,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>12</v>
       </c>
@@ -4604,7 +6509,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>7</v>
       </c>
@@ -4627,7 +6532,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>7</v>
       </c>
@@ -4652,5 +6557,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>